<commit_message>
Two excel file by negar, and updates on sensitivity module
</commit_message>
<xml_diff>
--- a/CVX_Kenya/Interventions/Sensitivity_try.xlsx
+++ b/CVX_Kenya/Interventions/Sensitivity_try.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gollinucci\Documents\GitHub\CIVICS_Kenya\CVX_Kenya\Interventions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amin\Documents\GitHub\My Kenya\CVX_Kenya\Interventions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B07AE07-ECC1-48C4-A514-724079E614C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309027C3-0D80-4FE9-B5D2-89CB6BB6830D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4170" yWindow="-21720" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S" sheetId="7" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="242">
   <si>
     <t>level_row</t>
   </si>
@@ -1049,7 +1049,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1371,16 +1373,16 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="1"/>
-    <col min="2" max="2" width="22.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="35.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="22.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1394,7 +1396,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1412,16 +1414,16 @@
         <v>-2.8687499999999998E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
     </row>
   </sheetData>
@@ -1442,15 +1444,15 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="33" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.109375" style="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1458,7 +1460,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1470,7 +1472,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1482,16 +1484,16 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
     </row>
   </sheetData>
@@ -1515,26 +1517,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="1"/>
-    <col min="2" max="2" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" style="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
     <col min="8" max="8" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.109375" style="1"/>
+    <col min="9" max="9" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1553,23 +1555,23 @@
       <c r="G1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1592,14 +1594,14 @@
         <f>-main!C26</f>
         <v>-6.7500000000000001E-5</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="J2" s="45" t="s">
-        <v>241</v>
+      <c r="I2" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="J2" s="45">
+        <v>0.12</v>
       </c>
       <c r="K2" s="45" t="s">
         <v>241</v>
@@ -1608,7 +1610,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1631,33 +1633,33 @@
         <f>main!C27</f>
         <v>6.7628632499999994E-2</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="J3" s="45" t="s">
-        <v>241</v>
-      </c>
-      <c r="K3" s="45" t="s">
-        <v>241</v>
-      </c>
-      <c r="L3" s="45" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I3" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="J3" s="45">
+        <v>0.06</v>
+      </c>
+      <c r="K3" s="45">
+        <v>0.1</v>
+      </c>
+      <c r="L3" s="45">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="2"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="2"/>
       <c r="D6" s="2"/>
@@ -1705,17 +1707,17 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="29" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1735,7 +1737,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1759,16 +1761,16 @@
         <v>222</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
     </row>
   </sheetData>
@@ -1810,14 +1812,14 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="56.88671875" customWidth="1"/>
-    <col min="3" max="3" width="47.109375" customWidth="1"/>
+    <col min="2" max="2" width="56.85546875" customWidth="1"/>
+    <col min="3" max="3" width="47.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>13</v>
       </c>
@@ -1829,7 +1831,7 @@
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1840,7 +1842,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1851,7 +1853,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1862,7 +1864,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1873,7 +1875,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1884,7 +1886,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1895,7 +1897,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1906,7 +1908,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1917,7 +1919,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1928,7 +1930,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1939,7 +1941,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1950,7 +1952,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1961,7 +1963,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1972,7 +1974,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1983,7 +1985,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1994,7 +1996,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -2005,7 +2007,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -2016,7 +2018,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -2027,7 +2029,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -2038,7 +2040,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -2049,7 +2051,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -2060,7 +2062,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -2071,7 +2073,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -2082,7 +2084,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -2093,7 +2095,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -2104,7 +2106,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -2115,7 +2117,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -2126,7 +2128,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -2137,7 +2139,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -2148,7 +2150,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -2159,7 +2161,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -2170,7 +2172,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -2181,7 +2183,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -2192,7 +2194,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>46</v>
       </c>
@@ -2203,7 +2205,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>47</v>
       </c>
@@ -2214,7 +2216,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>48</v>
       </c>
@@ -2225,7 +2227,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>49</v>
       </c>
@@ -2233,7 +2235,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>50</v>
       </c>
@@ -2241,7 +2243,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>51</v>
       </c>
@@ -2249,7 +2251,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -2257,7 +2259,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>53</v>
       </c>
@@ -2265,7 +2267,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>54</v>
       </c>
@@ -2273,7 +2275,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>55</v>
       </c>
@@ -2281,7 +2283,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>56</v>
       </c>
@@ -2289,7 +2291,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>57</v>
       </c>
@@ -2297,7 +2299,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>58</v>
       </c>
@@ -2305,7 +2307,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>59</v>
       </c>
@@ -2313,7 +2315,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>60</v>
       </c>
@@ -2321,7 +2323,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>61</v>
       </c>
@@ -2329,7 +2331,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>62</v>
       </c>
@@ -2337,7 +2339,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>63</v>
       </c>
@@ -2345,7 +2347,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>64</v>
       </c>
@@ -2353,7 +2355,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>65</v>
       </c>
@@ -2361,7 +2363,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>66</v>
       </c>
@@ -2369,87 +2371,87 @@
         <v>135</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>83</v>
       </c>
@@ -2463,22 +2465,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="81.6640625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" style="11" customWidth="1"/>
+    <col min="2" max="2" width="81.7109375" style="10" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="57.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="57.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="15" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>174</v>
       </c>
@@ -2501,7 +2503,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="41" t="s">
         <v>172</v>
       </c>
@@ -2518,7 +2520,7 @@
       <c r="F2" s="18"/>
       <c r="G2" s="18"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="42"/>
       <c r="B3" s="17" t="s">
         <v>173</v>
@@ -2533,7 +2535,7 @@
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="42"/>
       <c r="B4" s="17" t="s">
         <v>188</v>
@@ -2548,7 +2550,7 @@
       <c r="F4" s="18"/>
       <c r="G4" s="18"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="42"/>
       <c r="B5" s="17" t="s">
         <v>189</v>
@@ -2563,7 +2565,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="42"/>
       <c r="B6" s="17" t="s">
         <v>191</v>
@@ -2576,7 +2578,7 @@
       <c r="F6" s="18"/>
       <c r="G6" s="18"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="42"/>
       <c r="B7" s="17" t="s">
         <v>194</v>
@@ -2591,7 +2593,7 @@
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="42"/>
       <c r="B8" s="17" t="s">
         <v>198</v>
@@ -2606,7 +2608,7 @@
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="42"/>
       <c r="B9" s="17" t="s">
         <v>201</v>
@@ -2619,7 +2621,7 @@
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="42"/>
       <c r="B10" s="17" t="s">
         <v>200</v>
@@ -2634,7 +2636,7 @@
       <c r="F10" s="18"/>
       <c r="G10" s="18"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="42"/>
       <c r="B11" s="17" t="s">
         <v>207</v>
@@ -2649,7 +2651,7 @@
       <c r="F11" s="18"/>
       <c r="G11" s="18"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="42"/>
       <c r="B12" s="17" t="s">
         <v>209</v>
@@ -2664,7 +2666,7 @@
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="42"/>
       <c r="B13" s="17" t="s">
         <v>210</v>
@@ -2681,7 +2683,7 @@
       <c r="F13" s="18"/>
       <c r="G13" s="18"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="42"/>
       <c r="B14" s="17" t="s">
         <v>186</v>
@@ -2694,7 +2696,7 @@
       <c r="F14" s="18"/>
       <c r="G14" s="18"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="42"/>
       <c r="B15" s="17" t="s">
         <v>231</v>
@@ -2709,7 +2711,7 @@
       <c r="F15" s="18"/>
       <c r="G15" s="18"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="42"/>
       <c r="B16" s="30" t="s">
         <v>230</v>
@@ -2722,7 +2724,7 @@
       <c r="F16" s="18"/>
       <c r="G16" s="18"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="44" t="s">
         <v>180</v>
       </c>
@@ -2737,7 +2739,7 @@
       <c r="F17" s="21"/>
       <c r="G17" s="21"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="44"/>
       <c r="B18" s="16" t="s">
         <v>228</v>
@@ -2750,7 +2752,7 @@
       <c r="F18" s="21"/>
       <c r="G18" s="21"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="43" t="s">
         <v>181</v>
       </c>
@@ -2768,7 +2770,7 @@
       <c r="F19" s="23"/>
       <c r="G19" s="23"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="43"/>
       <c r="B20" s="29" t="s">
         <v>229</v>
@@ -2782,7 +2784,7 @@
       <c r="F20" s="23"/>
       <c r="G20" s="23"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="43"/>
       <c r="B21" s="29" t="s">
         <v>185</v>
@@ -2796,7 +2798,7 @@
       <c r="F21" s="23"/>
       <c r="G21" s="23"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="43"/>
       <c r="B22" s="22" t="s">
         <v>204</v>
@@ -2812,7 +2814,7 @@
       <c r="F22" s="23"/>
       <c r="G22" s="23"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="43"/>
       <c r="B23" s="22" t="s">
         <v>206</v>
@@ -2828,7 +2830,7 @@
       <c r="F23" s="23"/>
       <c r="G23" s="23"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="40" t="s">
         <v>182</v>
       </c>
@@ -2848,7 +2850,7 @@
       </c>
       <c r="G24" s="20"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="40"/>
       <c r="B25" s="19" t="s">
         <v>184</v>
@@ -2866,7 +2868,7 @@
       </c>
       <c r="G25" s="20"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="40"/>
       <c r="B26" s="19" t="s">
         <v>185</v>
@@ -2884,7 +2886,7 @@
       </c>
       <c r="G26" s="20"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="40"/>
       <c r="B27" s="19" t="s">
         <v>192</v>
@@ -2902,7 +2904,7 @@
       </c>
       <c r="G27" s="20"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="40"/>
       <c r="B28" s="19" t="s">
         <v>233</v>
@@ -2920,7 +2922,7 @@
       </c>
       <c r="G28" s="20"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="40"/>
       <c r="B29" s="19" t="s">
         <v>193</v>
@@ -2938,12 +2940,12 @@
       </c>
       <c r="G29" s="20"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" s="28" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="10" t="s">
         <v>218</v>
       </c>

</xml_diff>